<commit_message>
edits for JWM revision.  changed gamma to phi to avoid confusion with "y".  This was done in the text and sup info, but not the actual model code!
</commit_message>
<xml_diff>
--- a/VIT_Interval_thru2014b.xlsx
+++ b/VIT_Interval_thru2014b.xlsx
@@ -7,12 +7,12 @@
     <workbookView xWindow="2115" yWindow="180" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="for R" sheetId="2" r:id="rId1"/>
+    <sheet name="for stat analysis" sheetId="2" r:id="rId1"/>
     <sheet name="1-769" sheetId="3" r:id="rId2"/>
     <sheet name="770-825" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'for R'!$A$1:$K$576</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'for stat analysis'!$A$1:$K$576</definedName>
     <definedName name="VIT_Interval_4">#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -4810,7 +4810,7 @@
   <dimension ref="A1:N576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28728,7 +28728,7 @@
         <v>41784</v>
       </c>
       <c r="N533" s="23">
-        <f t="shared" ref="N533:N596" si="7">M533-G533</f>
+        <f t="shared" ref="N533:N576" si="7">M533-G533</f>
         <v>1</v>
       </c>
     </row>
@@ -30685,7 +30685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G532"/>
   <sheetViews>
-    <sheetView topLeftCell="A469" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A474" sqref="A474:XFD474"/>
     </sheetView>
   </sheetViews>
@@ -42946,7 +42946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>

</xml_diff>